<commit_message>
se cambiaron los alterts
</commit_message>
<xml_diff>
--- a/ui/tests/usability/Pruebas de usabilidad.xlsx
+++ b/ui/tests/usability/Pruebas de usabilidad.xlsx
@@ -5,23 +5,25 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jm.munoz14\Team01-front\ui\tests\usability\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="test 1" sheetId="1" r:id="rId1"/>
-    <sheet name="test 2" sheetId="2" r:id="rId2"/>
-    <sheet name="test 3" sheetId="5" r:id="rId3"/>
-    <sheet name="test 4" sheetId="4" r:id="rId4"/>
-    <sheet name="test 5" sheetId="9" r:id="rId5"/>
-    <sheet name="test 6" sheetId="8" r:id="rId6"/>
-    <sheet name="test 7" sheetId="7" r:id="rId7"/>
-    <sheet name="test 8" sheetId="6" r:id="rId8"/>
-    <sheet name="test 9" sheetId="11" r:id="rId9"/>
-    <sheet name="test 10" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja1" sheetId="12" r:id="rId2"/>
+    <sheet name="test 2" sheetId="2" r:id="rId3"/>
+    <sheet name="test 3" sheetId="5" r:id="rId4"/>
+    <sheet name="test 4" sheetId="4" r:id="rId5"/>
+    <sheet name="test 5" sheetId="9" r:id="rId6"/>
+    <sheet name="test 6" sheetId="8" r:id="rId7"/>
+    <sheet name="test 7" sheetId="7" r:id="rId8"/>
+    <sheet name="test 8" sheetId="6" r:id="rId9"/>
+    <sheet name="test 9" sheetId="11" r:id="rId10"/>
+    <sheet name="test 10" sheetId="10" r:id="rId11"/>
+    <sheet name="test 11" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="20">
   <si>
     <t>Tareas y preguntas</t>
   </si>
@@ -90,12 +92,15 @@
   </si>
   <si>
     <t>Daniel Felipe Moreno</t>
+  </si>
+  <si>
+    <t>Orlando Sabogal Rojas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,8 +418,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +506,98 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja10"/>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:E11"/>
@@ -592,7 +689,110 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E11"/>
@@ -684,7 +884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:E11"/>
@@ -776,7 +976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E11"/>
@@ -868,7 +1068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:E11"/>
@@ -960,7 +1160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:E11"/>
@@ -1052,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:E11"/>
@@ -1144,7 +1344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:E11"/>
@@ -1234,96 +1434,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja10"/>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:E7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>